<commit_message>
Update Tasks;minor fix for dropdown-menu responsive
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saocu\Desktop\Cybersoft - BC51\Bai tap\Nop bai\Capstone_JS_Nhom5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7AEA50-C3E8-4721-A72B-FA7C3AE10CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D275AFB3-D3FF-4AA5-8236-F0D46CCDE44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{9859029C-D30C-41D5-81E4-E6DB4BED5778}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -60,7 +60,31 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Nhật kha</t>
+    <t>Index page</t>
+  </si>
+  <si>
+    <t>HTML &amp; CSS</t>
+  </si>
+  <si>
+    <t>Admin Page</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsive </t>
+  </si>
+  <si>
+    <t>Add/Del/Update function</t>
+  </si>
+  <si>
+    <t>Search/Filter function</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Nhật Kha</t>
   </si>
 </sst>
 </file>
@@ -156,7 +180,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -299,11 +323,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -370,6 +431,42 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -685,14 +782,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2624A084-BDD8-4BC5-AA00-15653D921CC8}">
-  <dimension ref="A2:J16"/>
+  <dimension ref="A2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" customWidth="1"/>
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
@@ -732,7 +830,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
@@ -744,7 +844,7 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="15"/>
@@ -756,111 +856,197 @@
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="16"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="15"/>
       <c r="I6" s="21"/>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="10"/>
+      <c r="A7" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="14">
+        <v>45128</v>
+      </c>
+      <c r="C7" s="14">
+        <v>45135</v>
+      </c>
+      <c r="D7" s="30">
+        <v>1</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>17</v>
+      </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="21"/>
+      <c r="G7" s="16">
+        <v>45137</v>
+      </c>
+      <c r="H7" s="15">
+        <v>1</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>17</v>
+      </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="7"/>
+    <row r="8" spans="1:10" s="28" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="29">
+        <v>45128</v>
+      </c>
+      <c r="C8" s="29">
+        <v>45129</v>
+      </c>
+      <c r="D8" s="30">
+        <v>1</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="34">
+        <v>45137</v>
+      </c>
+      <c r="H8" s="15">
+        <v>1</v>
+      </c>
+      <c r="I8" s="32"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="1:10" s="28" customFormat="1" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="29">
+        <v>45129</v>
+      </c>
+      <c r="C9" s="29">
+        <v>45130</v>
+      </c>
+      <c r="D9" s="30">
+        <v>1</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="34">
+        <v>45137</v>
+      </c>
+      <c r="H9" s="15">
+        <v>1</v>
+      </c>
+      <c r="I9" s="32"/>
+      <c r="J9" s="27"/>
+    </row>
+    <row r="10" spans="1:10" s="28" customFormat="1" ht="24" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="29">
+        <v>45131</v>
+      </c>
+      <c r="C10" s="29">
+        <v>45132</v>
+      </c>
+      <c r="D10" s="30">
+        <v>1</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="29">
+        <v>45137</v>
+      </c>
+      <c r="H10" s="15">
+        <v>1</v>
+      </c>
+      <c r="I10" s="32"/>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:10" s="28" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="29">
+        <v>45132</v>
+      </c>
+      <c r="C11" s="29">
+        <v>45135</v>
+      </c>
+      <c r="D11" s="30">
+        <v>1</v>
+      </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="34">
+        <v>45137</v>
+      </c>
+      <c r="H11" s="15">
+        <v>1</v>
+      </c>
+      <c r="I11" s="32"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:10" s="28" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="29">
+        <v>45135</v>
+      </c>
+      <c r="C12" s="29">
+        <v>45135</v>
+      </c>
+      <c r="D12" s="30">
+        <v>1</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="29">
+        <v>45137</v>
+      </c>
+      <c r="H12" s="15">
+        <v>1</v>
+      </c>
+      <c r="I12" s="32"/>
+      <c r="J12" s="27"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="10"/>
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="14">
+        <v>45136</v>
+      </c>
+      <c r="C13" s="14">
+        <v>45137</v>
+      </c>
+      <c r="D13" s="30">
+        <v>1</v>
+      </c>
+      <c r="E13" s="33"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="21"/>
+      <c r="G13" s="14">
+        <v>45137</v>
+      </c>
+      <c r="H13" s="15">
+        <v>1</v>
+      </c>
+      <c r="I13" s="33"/>
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
-      <c r="D14" s="20"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11"/>
-      <c r="G14" s="16"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="15"/>
       <c r="I14" s="21"/>
       <c r="J14" s="7"/>
@@ -869,27 +1055,55 @@
       <c r="A15" s="6"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="16"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="15"/>
       <c r="I15" s="21"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="9"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E7:E13"/>
+    <mergeCell ref="I7:I13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>